<commit_message>
load pars, add ranges
</commit_message>
<xml_diff>
--- a/tests/databooks/programdata_sir.xlsx
+++ b/tests/databooks/programdata_sir.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="24940" windowHeight="13400"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="24940" windowHeight="13400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
   <si>
     <t>Populations &amp; programs</t>
   </si>
@@ -164,6 +164,30 @@
   </si>
   <si>
     <t>Value for a person covered by this program alone:</t>
+  </si>
+  <si>
+    <t>transpercontact</t>
+  </si>
+  <si>
+    <t>contacts</t>
+  </si>
+  <si>
+    <t>recrate</t>
+  </si>
+  <si>
+    <t>infdeath</t>
+  </si>
+  <si>
+    <t>susdeath</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -328,7 +352,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -389,6 +413,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -702,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1342,24 +1369,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
     <col min="3" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="2.6640625" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.83203125" customWidth="1"/>
     <col min="8" max="8" width="2.33203125" customWidth="1"/>
     <col min="9" max="13" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>27</v>
       </c>
       <c r="E1" s="12"/>
@@ -1370,7 +1401,7 @@
       <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:21" ht="40" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="20" t="s">
         <v>39</v>
       </c>
@@ -1407,7 +1438,6 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
       <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
@@ -1417,7 +1447,9 @@
       <c r="D3" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="25" t="s">
+        <v>50</v>
+      </c>
       <c r="F3" s="21">
         <v>0.01</v>
       </c>
@@ -1438,285 +1470,269 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4"/>
-      <c r="B4"/>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B4" s="15"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-    </row>
-    <row r="5" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="E4" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="21">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G4" s="21">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="K4" s="21">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B5" s="15"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="21">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G5" s="21">
+        <v>1.5E-3</v>
+      </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="20"/>
-      <c r="N5"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>28</v>
-      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="K5" s="21">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+    </row>
+    <row r="6" spans="1:21" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="20"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
       <c r="M6" s="22"/>
-      <c r="O6" s="19"/>
-    </row>
-    <row r="7" spans="1:21" ht="40" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="C7" s="20" t="s">
+      <c r="N6"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+    </row>
+    <row r="7" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="20"/>
+      <c r="N7"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="O8" s="19"/>
+    </row>
+    <row r="9" spans="1:21" ht="40" x14ac:dyDescent="0.2">
+      <c r="B9" s="14"/>
+      <c r="C9" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G9" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20" t="str">
+      <c r="H9" s="20"/>
+      <c r="I9" s="20" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Risk avoidance</v>
       </c>
-      <c r="J7" s="20" t="str">
+      <c r="J9" s="20" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Harm reduction 1</v>
       </c>
-      <c r="K7" s="20" t="str">
+      <c r="K9" s="20" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Harm reduction 2</v>
       </c>
-      <c r="L7" s="20" t="str">
+      <c r="L9" s="20" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Treatment 1</v>
       </c>
-      <c r="M7" s="20" t="str">
+      <c r="M9" s="20" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Treatment 2</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15" t="s">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21">
+      <c r="E10" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="21">
         <v>100</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G10" s="21">
         <v>10</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21">
+      <c r="H10" s="20"/>
+      <c r="I10" s="21">
         <v>15</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21">
+      <c r="J10" s="21"/>
+      <c r="K10" s="21">
         <v>20</v>
       </c>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="O8" t="s">
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="O10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-    </row>
-    <row r="10" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="20"/>
-      <c r="N10"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-    </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="E11" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="21">
+        <v>120</v>
+      </c>
+      <c r="G11" s="21">
+        <v>5</v>
+      </c>
       <c r="H11" s="20"/>
-      <c r="I11" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="O11" s="19"/>
-    </row>
-    <row r="12" spans="1:21" ht="40" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="C12" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>37</v>
+      <c r="I11" s="21">
+        <v>10</v>
+      </c>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B12" s="15"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="21">
+        <v>90</v>
+      </c>
+      <c r="G12" s="21">
+        <v>15</v>
       </c>
       <c r="H12" s="20"/>
-      <c r="I12" s="20" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
-        <v>Risk avoidance</v>
-      </c>
-      <c r="J12" s="20" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
-        <v>Harm reduction 1</v>
-      </c>
-      <c r="K12" s="20" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>Harm reduction 2</v>
-      </c>
-      <c r="L12" s="20" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>Treatment 1</v>
-      </c>
-      <c r="M12" s="20" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>Treatment 2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21">
-        <v>8</v>
-      </c>
-      <c r="G13" s="21">
-        <v>3</v>
-      </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21">
-        <v>4</v>
-      </c>
-      <c r="M13" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
+      <c r="I12" s="21">
+        <v>20</v>
+      </c>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+    </row>
+    <row r="13" spans="1:21" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B13"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+    </row>
+    <row r="14" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="12"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="20"/>
       <c r="N14"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
@@ -1726,151 +1742,144 @@
       <c r="T14" s="17"/>
       <c r="U14" s="17"/>
     </row>
-    <row r="15" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="20"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="20"/>
-      <c r="N15"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="I15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="O15" s="19"/>
+    </row>
+    <row r="16" spans="1:21" ht="40" x14ac:dyDescent="0.2">
+      <c r="B16" s="14"/>
+      <c r="C16" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="E16" s="20"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="F16" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="H16" s="20"/>
-      <c r="I16" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="O16" s="19"/>
-    </row>
-    <row r="17" spans="1:21" ht="40" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="C17" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20" t="str">
+      <c r="I16" s="20" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Risk avoidance</v>
       </c>
-      <c r="J17" s="20" t="str">
+      <c r="J16" s="20" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Harm reduction 1</v>
       </c>
-      <c r="K17" s="20" t="str">
+      <c r="K16" s="20" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Harm reduction 2</v>
       </c>
-      <c r="L17" s="20" t="str">
+      <c r="L16" s="20" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Treatment 1</v>
       </c>
-      <c r="M17" s="20" t="str">
+      <c r="M16" s="20" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Treatment 2</v>
       </c>
     </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B17" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="21">
+        <v>8</v>
+      </c>
+      <c r="G17" s="21">
+        <v>3</v>
+      </c>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21">
+        <v>4</v>
+      </c>
+      <c r="M17" s="21">
+        <v>4</v>
+      </c>
+    </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="20"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="25" t="s">
+        <v>51</v>
+      </c>
       <c r="F18" s="21">
-        <v>0.02</v>
-      </c>
-      <c r="G18" s="21">
-        <v>0.01</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G18" s="21"/>
       <c r="H18" s="20"/>
       <c r="I18" s="21"/>
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
-      <c r="L18" s="21">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="M18" s="21">
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19"/>
-      <c r="B19"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B19" s="15"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="17"/>
-    </row>
-    <row r="20" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="20"/>
+      <c r="E19" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="21">
+        <v>10</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+    </row>
+    <row r="20" spans="1:21" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
       <c r="N20"/>
       <c r="O20" s="17"/>
       <c r="P20" s="17"/>
@@ -1880,92 +1889,314 @@
       <c r="T20" s="17"/>
       <c r="U20" s="17"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+    <row r="21" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="12"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="20"/>
+      <c r="N21"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="O21" s="19"/>
-    </row>
-    <row r="22" spans="1:21" ht="40" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="C22" s="20" t="s">
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="O22" s="19"/>
+    </row>
+    <row r="23" spans="1:21" ht="40" x14ac:dyDescent="0.2">
+      <c r="B23" s="14"/>
+      <c r="C23" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D23" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20" t="s">
+      <c r="E23" s="20"/>
+      <c r="F23" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G23" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20" t="str">
+      <c r="H23" s="20"/>
+      <c r="I23" s="20" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Risk avoidance</v>
       </c>
-      <c r="J22" s="20" t="str">
+      <c r="J23" s="20" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Harm reduction 1</v>
       </c>
-      <c r="K22" s="20" t="str">
+      <c r="K23" s="20" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Harm reduction 2</v>
       </c>
-      <c r="L22" s="20" t="str">
+      <c r="L23" s="20" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Treatment 1</v>
       </c>
-      <c r="M22" s="20" t="str">
+      <c r="M23" s="20" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Treatment 2</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15" t="s">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B24" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C24" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="21">
+        <v>0.02</v>
+      </c>
+      <c r="G24" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="H24" s="20"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M24" s="21">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B25" s="15"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B26" s="15"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+    </row>
+    <row r="27" spans="1:21" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+    </row>
+    <row r="28" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="12"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="20"/>
+      <c r="N28"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="O29" s="19"/>
+    </row>
+    <row r="30" spans="1:21" ht="40" x14ac:dyDescent="0.2">
+      <c r="A30" s="14"/>
+      <c r="C30" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>Risk avoidance</v>
+      </c>
+      <c r="J30" s="20" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>Harm reduction 1</v>
+      </c>
+      <c r="K30" s="20" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>Harm reduction 2</v>
+      </c>
+      <c r="L30" s="20" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>Treatment 1</v>
+      </c>
+      <c r="M30" s="20" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Treatment 2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D31" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="O23" t="s">
+      <c r="E31" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="O31" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="E32" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="E33" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8 C13 C18 C3 C23">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3 C10 C17 C24 C31">
       <formula1>"Random,Nested,Additive"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D3 D8 D13 D18 D23">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D24 D3 D10 D17 D31">
       <formula1>"Synergistic,Best"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>